<commit_message>
EPICP-1 added ident to DD_EPICP_TRACY
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{06535FC6-E1C6-4A3F-86FF-05399DCBACA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CD5EB413-990C-4E12-BD5F-C0558CA62A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="131">
   <si>
     <t>index</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>Graduation 8th grade</t>
+  </si>
+  <si>
+    <t>ident</t>
+  </si>
+  <si>
+    <t>participant identifier</t>
   </si>
 </sst>
 </file>
@@ -819,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,12 +851,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -858,32 +865,32 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -891,32 +898,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -924,10 +931,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -935,10 +942,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>47</v>
@@ -946,10 +953,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -957,32 +964,32 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -990,10 +997,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1001,10 +1008,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
@@ -1012,10 +1019,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1023,10 +1030,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
@@ -1034,10 +1041,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -1045,10 +1052,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -1056,10 +1063,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -1067,10 +1074,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
@@ -1078,10 +1085,10 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>47</v>
@@ -1089,10 +1096,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
@@ -1100,10 +1107,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
@@ -1111,10 +1118,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
@@ -1122,32 +1129,32 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>73</v>
       </c>
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>74</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
@@ -1155,166 +1162,177 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>34</v>
+      <c r="B32" t="s">
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="D34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>79</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>78</v>
       </c>
-      <c r="D36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>39</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>81</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>83</v>
       </c>
-      <c r="D38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>82</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>85</v>
       </c>
-      <c r="D40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
-      </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>44</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>86</v>
       </c>
-      <c r="D42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>87</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>88</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1328,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adjusting DD and DPE for EPICP according to provided dataset
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A2A608-BC0C-420A-BF46-04199B43F7C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FCEB83-04DD-4F4D-94B1-8BA2ABB54D4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="128">
   <si>
     <t>index</t>
   </si>
@@ -53,15 +53,6 @@
     <t>occstat6</t>
   </si>
   <si>
-    <t>ZR3</t>
-  </si>
-  <si>
-    <t>PF3</t>
-  </si>
-  <si>
-    <t>ZT3</t>
-  </si>
-  <si>
     <t>ysmkces0</t>
   </si>
   <si>
@@ -393,6 +384,27 @@
   </si>
   <si>
     <t>pal</t>
+  </si>
+  <si>
+    <t>zt3</t>
+  </si>
+  <si>
+    <t>zr3</t>
+  </si>
+  <si>
+    <t>pf3</t>
+  </si>
+  <si>
+    <t>prevalent</t>
+  </si>
+  <si>
+    <t>incident (not verif.)</t>
+  </si>
+  <si>
+    <t>incident I15</t>
+  </si>
+  <si>
+    <t>inc. Diabetes (other types)</t>
   </si>
 </sst>
 </file>
@@ -807,7 +819,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,24 +845,24 @@
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,10 +870,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,32 +881,32 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,10 +914,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -913,362 +925,362 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" t="s">
         <v>39</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1279,15 +1291,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1305,24 +1317,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1344,7 +1356,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1355,7 +1367,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1377,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1388,7 +1400,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1399,62 +1411,62 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1476,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1509,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1520,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1542,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,392 +1565,524 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
         <v>5</v>
       </c>
-      <c r="C41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>24</v>
+      <c r="A43" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B44">
-        <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>29</v>
+      <c r="A50" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>31</v>
+      <c r="A51" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>31</v>
+      <c r="A52" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>33</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55">
         <v>2</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70">
         <v>2</v>
       </c>
-      <c r="C58" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59">
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71">
         <v>6</v>
       </c>
-      <c r="C59" t="s">
-        <v>110</v>
+      <c r="C71" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed ff10 from variable list in DD due to changed calculation of number of children
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DD5CD8-56C9-438E-A5D9-56AC194307E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9162F040-72D2-455E-95E7-AE97FA0A6AF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
   <si>
     <t>index</t>
   </si>
@@ -188,9 +188,6 @@
     <t>How many children have you born?</t>
   </si>
   <si>
-    <t>Total number of stillbirths</t>
-  </si>
-  <si>
     <t>How old were you when you gave birth to your first child?</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
   </si>
   <si>
     <t>d_recrui</t>
-  </si>
-  <si>
-    <t>ff10</t>
   </si>
   <si>
     <t>pal</t>
@@ -816,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +839,10 @@
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
         <v>115</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -856,7 +850,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -889,10 +883,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -900,7 +894,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -933,7 +927,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
@@ -944,7 +938,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -955,7 +949,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -966,7 +960,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -1043,7 +1037,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -1054,7 +1048,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -1065,7 +1059,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>57</v>
@@ -1076,7 +1070,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>58</v>
@@ -1086,8 +1080,8 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>19</v>
+      <c r="B24" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>59</v>
@@ -1097,8 +1091,8 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>20</v>
+      <c r="B25" t="s">
+        <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>60</v>
@@ -1109,18 +1103,18 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
         <v>62</v>
@@ -1130,21 +1124,21 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>22</v>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D29" t="s">
@@ -1152,134 +1146,123 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>76</v>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
       </c>
       <c r="D30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>26</v>
+      <c r="B31" t="s">
+        <v>27</v>
       </c>
       <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
         <v>66</v>
       </c>
-      <c r="D31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>29</v>
+      <c r="B34" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
         <v>69</v>
       </c>
-      <c r="D35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>34</v>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>35</v>
+      <c r="B40" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C40" t="s">
         <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1293,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,24 +1300,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1367,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1378,7 +1361,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1389,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1400,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1411,62 +1394,62 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1477,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1488,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1510,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1521,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1532,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1554,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1565,7 +1548,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1576,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1587,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1609,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1620,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1631,7 +1614,7 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1664,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1686,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1697,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1719,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1741,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1763,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,7 +1757,7 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1785,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1796,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1818,7 +1801,7 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,7 +1812,7 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1840,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1851,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1862,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1873,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1884,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1895,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1906,7 +1889,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1917,7 +1900,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1928,7 +1911,7 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1939,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1950,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1961,7 +1944,7 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1972,7 +1955,7 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1983,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1994,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2016,7 +1999,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2027,7 +2010,7 @@
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2038,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2049,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2060,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2071,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2082,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2093,7 +2076,7 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPICP-5 adjustments in the comment section
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA6EDCE-A432-4197-ADF4-0E955F0FC41F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4C15E-BB3E-4BA0-9252-0BEF85F39486}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="129">
   <si>
     <t>index</t>
   </si>
@@ -404,13 +404,10 @@
     <t>inccanc</t>
   </si>
   <si>
-    <t>incident first occuring cancer</t>
-  </si>
-  <si>
     <t>dcens_canc</t>
   </si>
   <si>
-    <t>censored age for cancer at FUP5</t>
+    <t>censored date for cancer at FUP5</t>
   </si>
 </sst>
 </file>
@@ -473,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,6 +489,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -830,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,8 +1230,8 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>32</v>
+      <c r="B36" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
@@ -1287,24 +1285,13 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
+      <c r="C41" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="D41" s="10" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>